<commit_message>
updated to work with GNRDIO Scan
</commit_message>
<xml_diff>
--- a/lighterFluid/heavierFluidOutputs/ptlBackConvert.xlsx
+++ b/lighterFluid/heavierFluidOutputs/ptlBackConvert.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27531"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\eoghanoc\source\repos\lighterFluid\lighterFluid\heavierFluidOutputs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cmichel1\source\repos\lighterFluid\lighterFluid\heavierFluidOutputs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{74D10BF4-3AA6-423A-B6C7-7E8C863BBCF7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{39584988-CDC4-40AE-904E-F03750EA7294}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17520" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38550" windowHeight="18480" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="arr_common" sheetId="1" r:id="rId1"/>
@@ -3781,13 +3781,16 @@
   <dimension ref="A1:BC443"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="3" ySplit="1" topLeftCell="D2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="1" topLeftCell="D167" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight"/>
+      <selection pane="bottomRight" activeCell="T1" sqref="T1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="20" max="20" width="13.42578125" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:55" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">

</xml_diff>